<commit_message>
status update and formatting
</commit_message>
<xml_diff>
--- a/RESULT  ANALYSIS.xlsx
+++ b/RESULT  ANALYSIS.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\stockanalysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/neerajkumar/stockanalysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{47D69455-1B93-47ED-B067-480F93175721}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9C5E434-C2D3-4E48-89F7-23C4D0F6D297}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D0B1D84E-FF7B-437F-827A-36FDC6E47B9C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26880" windowHeight="16800" xr2:uid="{D0B1D84E-FF7B-437F-827A-36FDC6E47B9C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$B$51</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -32,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="57">
   <si>
     <t>SYMBLE</t>
   </si>
@@ -49,21 +52,9 @@
     <t>WIPRO</t>
   </si>
   <si>
-    <t>pass</t>
-  </si>
-  <si>
     <t>HCLTECH</t>
   </si>
   <si>
-    <t>EX PASS</t>
-  </si>
-  <si>
-    <t>fail</t>
-  </si>
-  <si>
-    <t>Dmart</t>
-  </si>
-  <si>
     <t>HDFC BANK</t>
   </si>
   <si>
@@ -85,15 +76,6 @@
     <t>CRAFTSMAN</t>
   </si>
   <si>
-    <t>PASS</t>
-  </si>
-  <si>
-    <t>FAIL</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> EX PASS</t>
-  </si>
-  <si>
     <t>HINDUNILVR</t>
   </si>
   <si>
@@ -172,12 +154,6 @@
     <t>TVSMOTOR</t>
   </si>
   <si>
-    <t>ex fail</t>
-  </si>
-  <si>
-    <t>mix</t>
-  </si>
-  <si>
     <t>TATACONSUM</t>
   </si>
   <si>
@@ -214,7 +190,22 @@
     <t>SUPREMEIND</t>
   </si>
   <si>
-    <t>ex pass</t>
+    <t>P</t>
+  </si>
+  <si>
+    <t>EP</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>DMART</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>p</t>
   </si>
 </sst>
 </file>
@@ -566,19 +557,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D390358F-22BC-41BF-B31B-F4145C4653C1}">
-  <dimension ref="A1:B52"/>
+  <dimension ref="A1:B51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.77734375" customWidth="1"/>
+    <col min="1" max="1" width="25.83203125" customWidth="1"/>
     <col min="2" max="2" width="26.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -586,404 +577,412 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="B9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>9</v>
       </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="B13" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>15</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" t="s">
+      <c r="B18" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="B20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>20</v>
       </c>
-      <c r="B14" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="B21" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>21</v>
       </c>
-      <c r="B15" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="B22" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>22</v>
       </c>
-      <c r="B16" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="B23" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>23</v>
       </c>
-      <c r="B17" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="B24" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>24</v>
       </c>
-      <c r="B18" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>25</v>
-      </c>
-      <c r="B19" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="B26" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>26</v>
       </c>
-      <c r="B20" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+      <c r="B27" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>27</v>
       </c>
-      <c r="B21" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="B28" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>28</v>
       </c>
-      <c r="B22" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+      <c r="B29" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>29</v>
       </c>
-      <c r="B23" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="B30" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
         <v>30</v>
       </c>
-      <c r="B24" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+      <c r="B31" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
         <v>32</v>
       </c>
-      <c r="B25" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>31</v>
-      </c>
-      <c r="B26" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+      <c r="B33" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
         <v>33</v>
       </c>
-      <c r="B27" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+      <c r="B34" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
         <v>34</v>
       </c>
-      <c r="B28" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+      <c r="B35" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
         <v>35</v>
       </c>
-      <c r="B29" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+      <c r="B36" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
         <v>36</v>
       </c>
-      <c r="B30" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+      <c r="B37" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
         <v>37</v>
       </c>
-      <c r="B31" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
+      <c r="B38" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
         <v>38</v>
       </c>
-      <c r="B32" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+      <c r="B39" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
         <v>39</v>
       </c>
-      <c r="B33" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
+      <c r="B40" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
         <v>40</v>
       </c>
-      <c r="B34" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
+      <c r="B41" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
         <v>41</v>
       </c>
-      <c r="B35" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
+      <c r="B42" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
         <v>42</v>
       </c>
-      <c r="B36" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
+      <c r="B43" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
         <v>43</v>
       </c>
-      <c r="B37" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
+      <c r="B44" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
         <v>44</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B45" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>45</v>
-      </c>
-      <c r="B39" t="s">
+      <c r="B47" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
+      <c r="B48" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
         <v>48</v>
       </c>
-      <c r="B41" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
+      <c r="B49" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
         <v>49</v>
       </c>
-      <c r="B42" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
+      <c r="B50" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
         <v>50</v>
       </c>
-      <c r="B43" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>51</v>
-      </c>
-      <c r="B44" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>52</v>
-      </c>
-      <c r="B45" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>53</v>
-      </c>
-      <c r="B46" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>54</v>
-      </c>
-      <c r="B47" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>55</v>
-      </c>
-      <c r="B48" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>56</v>
-      </c>
-      <c r="B49" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>57</v>
-      </c>
-      <c r="B50" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>59</v>
-      </c>
-      <c r="B52" t="s">
-        <v>5</v>
+      <c r="B51" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:B51" xr:uid="{D390358F-22BC-41BF-B31B-F4145C4653C1}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B34">
+      <sortCondition ref="B1:B39"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
status update for reliance
</commit_message>
<xml_diff>
--- a/RESULT  ANALYSIS.xlsx
+++ b/RESULT  ANALYSIS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/neerajkumar/stockanalysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\stockanalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9C5E434-C2D3-4E48-89F7-23C4D0F6D297}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7C16F4F-DADE-43D4-8642-0D718B71362E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26880" windowHeight="16800" xr2:uid="{D0B1D84E-FF7B-437F-827A-36FDC6E47B9C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D0B1D84E-FF7B-437F-827A-36FDC6E47B9C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="57">
   <si>
     <t>SYMBLE</t>
   </si>
@@ -559,17 +559,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D390358F-22BC-41BF-B31B-F4145C4653C1}">
   <dimension ref="A1:B51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.83203125" customWidth="1"/>
+    <col min="1" max="1" width="25.77734375" customWidth="1"/>
     <col min="2" max="2" width="26.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -577,7 +577,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -585,7 +585,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -593,7 +593,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -601,7 +601,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -609,7 +609,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>54</v>
       </c>
@@ -617,7 +617,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -625,7 +625,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -633,7 +633,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -641,7 +641,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -649,7 +649,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -657,7 +657,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -665,7 +665,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -673,7 +673,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -681,7 +681,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -689,7 +689,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -697,7 +697,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -705,7 +705,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -713,7 +713,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -721,7 +721,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -729,7 +729,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -737,7 +737,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -745,7 +745,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -753,7 +753,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -761,7 +761,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -769,7 +769,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -777,7 +777,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -785,7 +785,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -793,7 +793,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -801,7 +801,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -809,7 +809,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -817,7 +817,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -825,7 +825,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -833,7 +833,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -841,7 +841,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -849,7 +849,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -857,7 +857,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -865,7 +865,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -873,7 +873,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -881,7 +881,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -889,7 +889,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -897,7 +897,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -905,7 +905,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -913,7 +913,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -921,7 +921,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -929,7 +929,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -937,7 +937,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -945,7 +945,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -953,7 +953,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -961,15 +961,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>49</v>
       </c>
-      <c r="B50" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>50</v>
       </c>

</xml_diff>